<commit_message>
Using correct abbreviated name for Wuhan sharpbelly bornavirus (WhSBV)
</commit_message>
<xml_diff>
--- a/tabular/core/borna-reference_feature_locations.xlsx
+++ b/tabular/core/borna-reference_feature_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA-ve/Bornaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D5F413-23A2-7447-83C2-2C016608B4E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3310842-37BA-034B-8D0A-BBB55D1A8C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="1620" windowWidth="23300" windowHeight="13420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,10 +113,10 @@
     <t>MG599939</t>
   </si>
   <si>
-    <t>REF_WSBV</t>
+    <t>Cultervirus</t>
   </si>
   <si>
-    <t>Cultervirus</t>
+    <t>REF_WhSBV</t>
   </si>
 </sst>
 </file>
@@ -5522,8 +5522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C37" sqref="A1:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6162,10 +6162,10 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
         <v>25</v>
-      </c>
-      <c r="C32" t="s">
-        <v>26</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>13</v>
@@ -6182,10 +6182,10 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
         <v>25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>26</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>14</v>
@@ -6202,10 +6202,10 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
         <v>25</v>
-      </c>
-      <c r="C34" t="s">
-        <v>26</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>15</v>
@@ -6222,10 +6222,10 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
         <v>25</v>
-      </c>
-      <c r="C35" t="s">
-        <v>26</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>16</v>
@@ -6242,10 +6242,10 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
         <v>25</v>
-      </c>
-      <c r="C36" t="s">
-        <v>26</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>17</v>
@@ -6262,10 +6262,10 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
         <v>25</v>
-      </c>
-      <c r="C37" t="s">
-        <v>26</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>18</v>

</xml_diff>